<commit_message>
Change type of feedback ciruit to show on LCD, remove VietnameseSign from Name to show on LCD
</commit_message>
<xml_diff>
--- a/Protocol.xlsx
+++ b/Protocol.xlsx
@@ -1567,6 +1567,93 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1656,93 +1743,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2033,7 +2033,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:AA76"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="X62" sqref="X62"/>
     </sheetView>
   </sheetViews>
@@ -2048,16 +2048,16 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
@@ -2098,16 +2098,16 @@
       <c r="C6" s="12">
         <v>0</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="D6" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="65" t="s">
+      <c r="E6" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="65"/>
-      <c r="I6" s="65"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="61"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
@@ -2119,12 +2119,12 @@
       <c r="C7" s="12">
         <v>1</v>
       </c>
-      <c r="D7" s="45"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="65"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="61"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -2136,88 +2136,88 @@
       <c r="C8" s="12">
         <v>0</v>
       </c>
-      <c r="D8" s="46"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="65"/>
-      <c r="H8" s="65"/>
-      <c r="I8" s="65"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="56"/>
-      <c r="C9" s="57"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="86"/>
       <c r="D9" s="22"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="52"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="80"/>
+      <c r="G9" s="80"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="81"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="48"/>
+      <c r="C10" s="77"/>
       <c r="D10" s="23"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="54"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="55"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="83"/>
+      <c r="H10" s="83"/>
+      <c r="I10" s="84"/>
     </row>
     <row r="11" spans="1:9" ht="3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="58"/>
-      <c r="C11" s="60"/>
+      <c r="B11" s="87"/>
+      <c r="C11" s="89"/>
       <c r="D11" s="24"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="55"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="83"/>
+      <c r="G11" s="83"/>
+      <c r="H11" s="83"/>
+      <c r="I11" s="84"/>
     </row>
     <row r="12" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="53"/>
-      <c r="C12" s="54"/>
+      <c r="B12" s="82"/>
+      <c r="C12" s="83"/>
       <c r="D12" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="55"/>
+      <c r="E12" s="83"/>
+      <c r="F12" s="83"/>
+      <c r="G12" s="83"/>
+      <c r="H12" s="83"/>
+      <c r="I12" s="84"/>
     </row>
     <row r="13" spans="1:9" ht="3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="53"/>
-      <c r="C13" s="55"/>
+      <c r="B13" s="82"/>
+      <c r="C13" s="84"/>
       <c r="D13" s="24"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="62"/>
-      <c r="I13" s="63"/>
+      <c r="E13" s="90"/>
+      <c r="F13" s="91"/>
+      <c r="G13" s="91"/>
+      <c r="H13" s="91"/>
+      <c r="I13" s="92"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="53"/>
-      <c r="C14" s="55"/>
+      <c r="B14" s="82"/>
+      <c r="C14" s="84"/>
       <c r="D14" s="25"/>
-      <c r="E14" s="47" t="s">
+      <c r="E14" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="48"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="78"/>
+      <c r="H14" s="78"/>
+      <c r="I14" s="77"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="53"/>
-      <c r="C15" s="55"/>
+      <c r="B15" s="82"/>
+      <c r="C15" s="84"/>
       <c r="D15" s="26"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="60"/>
+      <c r="E15" s="87"/>
+      <c r="F15" s="88"/>
+      <c r="G15" s="88"/>
+      <c r="H15" s="88"/>
+      <c r="I15" s="89"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="10"/>
@@ -2230,16 +2230,16 @@
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B17" s="64" t="s">
+      <c r="B17" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="64"/>
-      <c r="H17" s="64"/>
-      <c r="I17" s="64"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="62"/>
+      <c r="I17" s="62"/>
     </row>
     <row r="18" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B18" s="10"/>
@@ -2289,24 +2289,24 @@
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
-      <c r="J21" s="67"/>
-      <c r="K21" s="68"/>
-      <c r="L21" s="68"/>
-      <c r="M21" s="68"/>
-      <c r="N21" s="68"/>
-      <c r="O21" s="68"/>
-      <c r="P21" s="68"/>
-      <c r="Q21" s="68"/>
-      <c r="R21" s="68"/>
-      <c r="S21" s="68"/>
-      <c r="T21" s="68"/>
-      <c r="U21" s="68"/>
-      <c r="V21" s="68"/>
-      <c r="W21" s="68"/>
-      <c r="X21" s="68"/>
-      <c r="Y21" s="68"/>
-      <c r="Z21" s="68"/>
-      <c r="AA21" s="69"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="36"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="36"/>
+      <c r="Q21" s="36"/>
+      <c r="R21" s="36"/>
+      <c r="S21" s="36"/>
+      <c r="T21" s="36"/>
+      <c r="U21" s="36"/>
+      <c r="V21" s="36"/>
+      <c r="W21" s="36"/>
+      <c r="X21" s="36"/>
+      <c r="Y21" s="36"/>
+      <c r="Z21" s="36"/>
+      <c r="AA21" s="37"/>
     </row>
     <row r="22" spans="2:27" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B22" s="10"/>
@@ -2317,46 +2317,46 @@
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
-      <c r="J22" s="70"/>
-      <c r="K22" s="75"/>
-      <c r="L22" s="76" t="s">
+      <c r="J22" s="38"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="M22" s="76" t="s">
+      <c r="M22" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="N22" s="76"/>
-      <c r="O22" s="76" t="s">
+      <c r="N22" s="44"/>
+      <c r="O22" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="P22" s="76" t="s">
+      <c r="P22" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="Q22" s="76" t="s">
+      <c r="Q22" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="R22" s="76" t="s">
+      <c r="R22" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="S22" s="76" t="s">
+      <c r="S22" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="T22" s="76"/>
-      <c r="U22" s="76" t="s">
+      <c r="T22" s="44"/>
+      <c r="U22" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="V22" s="76" t="s">
+      <c r="V22" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="W22" s="76" t="s">
+      <c r="W22" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="X22" s="76" t="s">
+      <c r="X22" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="Y22" s="76"/>
-      <c r="Z22" s="77"/>
-      <c r="AA22" s="74"/>
+      <c r="Y22" s="44"/>
+      <c r="Z22" s="45"/>
+      <c r="AA22" s="42"/>
     </row>
     <row r="23" spans="2:27" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
@@ -2367,52 +2367,52 @@
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
-      <c r="J23" s="70"/>
-      <c r="K23" s="78"/>
-      <c r="L23" s="66" t="s">
+      <c r="J23" s="38"/>
+      <c r="K23" s="46"/>
+      <c r="L23" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="M23" s="66" t="s">
+      <c r="M23" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="N23" s="66" t="s">
+      <c r="N23" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="O23" s="66" t="s">
+      <c r="O23" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="P23" s="66" t="s">
+      <c r="P23" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="Q23" s="66" t="s">
+      <c r="Q23" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="R23" s="66" t="s">
+      <c r="R23" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="S23" s="66" t="s">
+      <c r="S23" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="T23" s="66" t="s">
+      <c r="T23" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="U23" s="66" t="s">
+      <c r="U23" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="V23" s="66" t="s">
+      <c r="V23" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="W23" s="66" t="s">
+      <c r="W23" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="X23" s="66" t="s">
+      <c r="X23" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="Y23" s="66" t="s">
+      <c r="Y23" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="Z23" s="79"/>
-      <c r="AA23" s="74"/>
+      <c r="Z23" s="47"/>
+      <c r="AA23" s="42"/>
     </row>
     <row r="24" spans="2:27" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B24" s="10"/>
@@ -2423,52 +2423,52 @@
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
-      <c r="J24" s="70"/>
-      <c r="K24" s="78"/>
-      <c r="L24" s="66" t="s">
+      <c r="J24" s="38"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="M24" s="66" t="s">
+      <c r="M24" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="N24" s="66" t="s">
+      <c r="N24" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="O24" s="66" t="s">
+      <c r="O24" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="P24" s="66">
+      <c r="P24" s="34">
         <v>9</v>
       </c>
-      <c r="Q24" s="66">
+      <c r="Q24" s="34">
         <v>8</v>
       </c>
-      <c r="R24" s="66" t="s">
+      <c r="R24" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="S24" s="66">
+      <c r="S24" s="34">
         <v>1</v>
       </c>
-      <c r="T24" s="66" t="s">
+      <c r="T24" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="U24" s="66">
+      <c r="U24" s="34">
         <v>0</v>
       </c>
-      <c r="V24" s="66">
+      <c r="V24" s="34">
         <v>0</v>
       </c>
-      <c r="W24" s="66">
+      <c r="W24" s="34">
         <v>0</v>
       </c>
-      <c r="X24" s="66">
+      <c r="X24" s="34">
         <v>0</v>
       </c>
-      <c r="Y24" s="66">
+      <c r="Y24" s="34">
         <v>0</v>
       </c>
-      <c r="Z24" s="79"/>
-      <c r="AA24" s="74"/>
+      <c r="Z24" s="47"/>
+      <c r="AA24" s="42"/>
     </row>
     <row r="25" spans="2:27" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="10"/>
@@ -2479,42 +2479,42 @@
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
       <c r="I25" s="10"/>
-      <c r="J25" s="70"/>
-      <c r="K25" s="80"/>
-      <c r="L25" s="81" t="s">
+      <c r="J25" s="38"/>
+      <c r="K25" s="48"/>
+      <c r="L25" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="M25" s="81" t="s">
+      <c r="M25" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="N25" s="81" t="s">
+      <c r="N25" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="O25" s="81"/>
-      <c r="P25" s="81">
+      <c r="O25" s="49"/>
+      <c r="P25" s="49">
         <v>5</v>
       </c>
-      <c r="Q25" s="81">
+      <c r="Q25" s="49">
         <v>0</v>
       </c>
-      <c r="R25" s="81">
+      <c r="R25" s="49">
         <v>0</v>
       </c>
-      <c r="S25" s="81">
+      <c r="S25" s="49">
         <v>0</v>
       </c>
-      <c r="T25" s="81">
+      <c r="T25" s="49">
         <v>0</v>
       </c>
-      <c r="U25" s="81">
+      <c r="U25" s="49">
         <v>0</v>
       </c>
-      <c r="V25" s="81"/>
-      <c r="W25" s="81"/>
-      <c r="X25" s="81"/>
-      <c r="Y25" s="81"/>
-      <c r="Z25" s="82"/>
-      <c r="AA25" s="74"/>
+      <c r="V25" s="49"/>
+      <c r="W25" s="49"/>
+      <c r="X25" s="49"/>
+      <c r="Y25" s="49"/>
+      <c r="Z25" s="50"/>
+      <c r="AA25" s="42"/>
     </row>
     <row r="26" spans="2:27" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="10"/>
@@ -2525,24 +2525,24 @@
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
-      <c r="J26" s="70"/>
-      <c r="K26" s="83"/>
-      <c r="L26" s="83"/>
-      <c r="M26" s="83"/>
-      <c r="N26" s="83"/>
-      <c r="O26" s="83"/>
-      <c r="P26" s="83"/>
-      <c r="Q26" s="83"/>
-      <c r="R26" s="83"/>
-      <c r="S26" s="83"/>
-      <c r="T26" s="83"/>
-      <c r="U26" s="83"/>
-      <c r="V26" s="83"/>
-      <c r="W26" s="83"/>
-      <c r="X26" s="83"/>
-      <c r="Y26" s="83"/>
-      <c r="Z26" s="83"/>
-      <c r="AA26" s="74"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="51"/>
+      <c r="L26" s="51"/>
+      <c r="M26" s="51"/>
+      <c r="N26" s="51"/>
+      <c r="O26" s="51"/>
+      <c r="P26" s="51"/>
+      <c r="Q26" s="51"/>
+      <c r="R26" s="51"/>
+      <c r="S26" s="51"/>
+      <c r="T26" s="51"/>
+      <c r="U26" s="51"/>
+      <c r="V26" s="51"/>
+      <c r="W26" s="51"/>
+      <c r="X26" s="51"/>
+      <c r="Y26" s="51"/>
+      <c r="Z26" s="51"/>
+      <c r="AA26" s="42"/>
     </row>
     <row r="27" spans="2:27" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="10"/>
@@ -2553,24 +2553,24 @@
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
       <c r="I27" s="10"/>
-      <c r="J27" s="71"/>
-      <c r="K27" s="84"/>
-      <c r="L27" s="84"/>
-      <c r="M27" s="84"/>
-      <c r="N27" s="84"/>
-      <c r="O27" s="84"/>
-      <c r="P27" s="84"/>
-      <c r="Q27" s="84"/>
-      <c r="R27" s="84"/>
-      <c r="S27" s="72"/>
-      <c r="T27" s="72"/>
-      <c r="U27" s="72"/>
-      <c r="V27" s="72"/>
-      <c r="W27" s="72"/>
-      <c r="X27" s="72"/>
-      <c r="Y27" s="72"/>
-      <c r="Z27" s="72"/>
-      <c r="AA27" s="73"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="52"/>
+      <c r="L27" s="52"/>
+      <c r="M27" s="52"/>
+      <c r="N27" s="52"/>
+      <c r="O27" s="52"/>
+      <c r="P27" s="52"/>
+      <c r="Q27" s="52"/>
+      <c r="R27" s="52"/>
+      <c r="S27" s="40"/>
+      <c r="T27" s="40"/>
+      <c r="U27" s="40"/>
+      <c r="V27" s="40"/>
+      <c r="W27" s="40"/>
+      <c r="X27" s="40"/>
+      <c r="Y27" s="40"/>
+      <c r="Z27" s="40"/>
+      <c r="AA27" s="41"/>
     </row>
     <row r="28" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B28" s="10"/>
@@ -2640,24 +2640,24 @@
       <c r="G33" s="11"/>
       <c r="H33" s="11"/>
       <c r="I33" s="11"/>
-      <c r="J33" s="67"/>
-      <c r="K33" s="68"/>
-      <c r="L33" s="68"/>
-      <c r="M33" s="68"/>
-      <c r="N33" s="68"/>
-      <c r="O33" s="68"/>
-      <c r="P33" s="68"/>
-      <c r="Q33" s="68"/>
-      <c r="R33" s="68"/>
-      <c r="S33" s="68"/>
-      <c r="T33" s="68"/>
-      <c r="U33" s="68"/>
-      <c r="V33" s="68"/>
-      <c r="W33" s="68"/>
-      <c r="X33" s="68"/>
-      <c r="Y33" s="68"/>
-      <c r="Z33" s="68"/>
-      <c r="AA33" s="69"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="36"/>
+      <c r="L33" s="36"/>
+      <c r="M33" s="36"/>
+      <c r="N33" s="36"/>
+      <c r="O33" s="36"/>
+      <c r="P33" s="36"/>
+      <c r="Q33" s="36"/>
+      <c r="R33" s="36"/>
+      <c r="S33" s="36"/>
+      <c r="T33" s="36"/>
+      <c r="U33" s="36"/>
+      <c r="V33" s="36"/>
+      <c r="W33" s="36"/>
+      <c r="X33" s="36"/>
+      <c r="Y33" s="36"/>
+      <c r="Z33" s="36"/>
+      <c r="AA33" s="37"/>
     </row>
     <row r="34" spans="2:27" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B34" s="11"/>
@@ -2668,48 +2668,48 @@
       <c r="G34" s="11"/>
       <c r="H34" s="11"/>
       <c r="I34" s="11"/>
-      <c r="J34" s="70"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="76" t="s">
+      <c r="J34" s="38"/>
+      <c r="K34" s="43"/>
+      <c r="L34" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="M34" s="76" t="s">
+      <c r="M34" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="N34" s="76" t="s">
+      <c r="N34" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="O34" s="76" t="s">
+      <c r="O34" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="P34" s="76"/>
-      <c r="Q34" s="76" t="s">
+      <c r="P34" s="44"/>
+      <c r="Q34" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="R34" s="76" t="s">
+      <c r="R34" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="S34" s="76" t="s">
+      <c r="S34" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="T34" s="76" t="s">
+      <c r="T34" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="U34" s="76" t="s">
+      <c r="U34" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="V34" s="76"/>
-      <c r="W34" s="76" t="s">
+      <c r="V34" s="44"/>
+      <c r="W34" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="X34" s="76" t="s">
+      <c r="X34" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="Y34" s="76" t="s">
+      <c r="Y34" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="Z34" s="77"/>
-      <c r="AA34" s="74"/>
+      <c r="Z34" s="45"/>
+      <c r="AA34" s="42"/>
     </row>
     <row r="35" spans="2:27" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B35" s="11"/>
@@ -2720,52 +2720,52 @@
       <c r="G35" s="11"/>
       <c r="H35" s="11"/>
       <c r="I35" s="11"/>
-      <c r="J35" s="70"/>
-      <c r="K35" s="78"/>
-      <c r="L35" s="66" t="s">
+      <c r="J35" s="38"/>
+      <c r="K35" s="46"/>
+      <c r="L35" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="M35" s="66" t="s">
+      <c r="M35" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="N35" s="66" t="s">
+      <c r="N35" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="O35" s="66" t="s">
+      <c r="O35" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="P35" s="66" t="s">
+      <c r="P35" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="Q35" s="66" t="s">
+      <c r="Q35" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="R35" s="66" t="s">
+      <c r="R35" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="S35" s="66" t="s">
+      <c r="S35" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="T35" s="66" t="s">
+      <c r="T35" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="U35" s="66" t="s">
+      <c r="U35" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="V35" s="66" t="s">
+      <c r="V35" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="W35" s="66" t="s">
+      <c r="W35" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="X35" s="66" t="s">
+      <c r="X35" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="Y35" s="66" t="s">
+      <c r="Y35" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="Z35" s="79"/>
-      <c r="AA35" s="74"/>
+      <c r="Z35" s="47"/>
+      <c r="AA35" s="42"/>
     </row>
     <row r="36" spans="2:27" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B36" s="11"/>
@@ -2776,52 +2776,52 @@
       <c r="G36" s="11"/>
       <c r="H36" s="11"/>
       <c r="I36" s="11"/>
-      <c r="J36" s="70"/>
-      <c r="K36" s="78"/>
-      <c r="L36" s="66" t="s">
+      <c r="J36" s="38"/>
+      <c r="K36" s="46"/>
+      <c r="L36" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="M36" s="66" t="s">
+      <c r="M36" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="N36" s="66" t="s">
+      <c r="N36" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="O36" s="66" t="s">
+      <c r="O36" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="P36" s="66">
+      <c r="P36" s="34">
         <v>9</v>
       </c>
-      <c r="Q36" s="66">
+      <c r="Q36" s="34">
         <v>8</v>
       </c>
-      <c r="R36" s="66" t="s">
+      <c r="R36" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="S36" s="66">
+      <c r="S36" s="34">
         <v>1</v>
       </c>
-      <c r="T36" s="66" t="s">
+      <c r="T36" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="U36" s="66">
+      <c r="U36" s="34">
         <v>0</v>
       </c>
-      <c r="V36" s="66">
+      <c r="V36" s="34">
         <v>0</v>
       </c>
-      <c r="W36" s="66">
+      <c r="W36" s="34">
         <v>0</v>
       </c>
-      <c r="X36" s="66">
+      <c r="X36" s="34">
         <v>0</v>
       </c>
-      <c r="Y36" s="66">
+      <c r="Y36" s="34">
         <v>0</v>
       </c>
-      <c r="Z36" s="79"/>
-      <c r="AA36" s="74"/>
+      <c r="Z36" s="47"/>
+      <c r="AA36" s="42"/>
     </row>
     <row r="37" spans="2:27" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="11"/>
@@ -2832,42 +2832,42 @@
       <c r="G37" s="11"/>
       <c r="H37" s="11"/>
       <c r="I37" s="11"/>
-      <c r="J37" s="70"/>
-      <c r="K37" s="80"/>
-      <c r="L37" s="81" t="s">
+      <c r="J37" s="38"/>
+      <c r="K37" s="48"/>
+      <c r="L37" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="M37" s="81" t="s">
+      <c r="M37" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="N37" s="81" t="s">
+      <c r="N37" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="O37" s="81"/>
-      <c r="P37" s="81">
+      <c r="O37" s="49"/>
+      <c r="P37" s="49">
         <v>5</v>
       </c>
-      <c r="Q37" s="81">
+      <c r="Q37" s="49">
         <v>0</v>
       </c>
-      <c r="R37" s="81">
+      <c r="R37" s="49">
         <v>0</v>
       </c>
-      <c r="S37" s="81">
+      <c r="S37" s="49">
         <v>0</v>
       </c>
-      <c r="T37" s="81">
+      <c r="T37" s="49">
         <v>0</v>
       </c>
-      <c r="U37" s="81">
+      <c r="U37" s="49">
         <v>0</v>
       </c>
-      <c r="V37" s="81"/>
-      <c r="W37" s="81"/>
-      <c r="X37" s="81"/>
-      <c r="Y37" s="81"/>
-      <c r="Z37" s="82"/>
-      <c r="AA37" s="74"/>
+      <c r="V37" s="49"/>
+      <c r="W37" s="49"/>
+      <c r="X37" s="49"/>
+      <c r="Y37" s="49"/>
+      <c r="Z37" s="50"/>
+      <c r="AA37" s="42"/>
     </row>
     <row r="38" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="11"/>
@@ -2878,24 +2878,24 @@
       <c r="G38" s="11"/>
       <c r="H38" s="11"/>
       <c r="I38" s="11"/>
-      <c r="J38" s="70"/>
-      <c r="K38" s="83"/>
-      <c r="L38" s="83"/>
-      <c r="M38" s="83"/>
-      <c r="N38" s="83"/>
-      <c r="O38" s="83"/>
-      <c r="P38" s="83"/>
-      <c r="Q38" s="83"/>
-      <c r="R38" s="83"/>
-      <c r="S38" s="83"/>
-      <c r="T38" s="83"/>
-      <c r="U38" s="83"/>
-      <c r="V38" s="83"/>
-      <c r="W38" s="83"/>
-      <c r="X38" s="83"/>
-      <c r="Y38" s="83"/>
-      <c r="Z38" s="83"/>
-      <c r="AA38" s="74"/>
+      <c r="J38" s="38"/>
+      <c r="K38" s="51"/>
+      <c r="L38" s="51"/>
+      <c r="M38" s="51"/>
+      <c r="N38" s="51"/>
+      <c r="O38" s="51"/>
+      <c r="P38" s="51"/>
+      <c r="Q38" s="51"/>
+      <c r="R38" s="51"/>
+      <c r="S38" s="51"/>
+      <c r="T38" s="51"/>
+      <c r="U38" s="51"/>
+      <c r="V38" s="51"/>
+      <c r="W38" s="51"/>
+      <c r="X38" s="51"/>
+      <c r="Y38" s="51"/>
+      <c r="Z38" s="51"/>
+      <c r="AA38" s="42"/>
     </row>
     <row r="39" spans="2:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="11"/>
@@ -2906,24 +2906,24 @@
       <c r="G39" s="11"/>
       <c r="H39" s="11"/>
       <c r="I39" s="11"/>
-      <c r="J39" s="71"/>
-      <c r="K39" s="84"/>
-      <c r="L39" s="84"/>
-      <c r="M39" s="84"/>
-      <c r="N39" s="84"/>
-      <c r="O39" s="84"/>
-      <c r="P39" s="84"/>
-      <c r="Q39" s="84"/>
-      <c r="R39" s="84"/>
-      <c r="S39" s="72"/>
-      <c r="T39" s="72"/>
-      <c r="U39" s="72"/>
-      <c r="V39" s="72"/>
-      <c r="W39" s="72"/>
-      <c r="X39" s="72"/>
-      <c r="Y39" s="72"/>
-      <c r="Z39" s="72"/>
-      <c r="AA39" s="73"/>
+      <c r="J39" s="39"/>
+      <c r="K39" s="52"/>
+      <c r="L39" s="52"/>
+      <c r="M39" s="52"/>
+      <c r="N39" s="52"/>
+      <c r="O39" s="52"/>
+      <c r="P39" s="52"/>
+      <c r="Q39" s="52"/>
+      <c r="R39" s="52"/>
+      <c r="S39" s="40"/>
+      <c r="T39" s="40"/>
+      <c r="U39" s="40"/>
+      <c r="V39" s="40"/>
+      <c r="W39" s="40"/>
+      <c r="X39" s="40"/>
+      <c r="Y39" s="40"/>
+      <c r="Z39" s="40"/>
+      <c r="AA39" s="41"/>
     </row>
     <row r="40" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B40" s="11"/>
@@ -2993,24 +2993,24 @@
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
       <c r="I45" s="11"/>
-      <c r="J45" s="67"/>
-      <c r="K45" s="68"/>
-      <c r="L45" s="68"/>
-      <c r="M45" s="68"/>
-      <c r="N45" s="68"/>
-      <c r="O45" s="68"/>
-      <c r="P45" s="68"/>
-      <c r="Q45" s="68"/>
-      <c r="R45" s="68"/>
-      <c r="S45" s="68"/>
-      <c r="T45" s="68"/>
-      <c r="U45" s="68"/>
-      <c r="V45" s="68"/>
-      <c r="W45" s="68"/>
-      <c r="X45" s="68"/>
-      <c r="Y45" s="68"/>
-      <c r="Z45" s="68"/>
-      <c r="AA45" s="69"/>
+      <c r="J45" s="35"/>
+      <c r="K45" s="36"/>
+      <c r="L45" s="36"/>
+      <c r="M45" s="36"/>
+      <c r="N45" s="36"/>
+      <c r="O45" s="36"/>
+      <c r="P45" s="36"/>
+      <c r="Q45" s="36"/>
+      <c r="R45" s="36"/>
+      <c r="S45" s="36"/>
+      <c r="T45" s="36"/>
+      <c r="U45" s="36"/>
+      <c r="V45" s="36"/>
+      <c r="W45" s="36"/>
+      <c r="X45" s="36"/>
+      <c r="Y45" s="36"/>
+      <c r="Z45" s="36"/>
+      <c r="AA45" s="37"/>
     </row>
     <row r="46" spans="2:27" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B46" s="11"/>
@@ -3021,44 +3021,44 @@
       <c r="G46" s="11"/>
       <c r="H46" s="11"/>
       <c r="I46" s="11"/>
-      <c r="J46" s="70"/>
-      <c r="K46" s="75"/>
-      <c r="L46" s="76" t="s">
+      <c r="J46" s="38"/>
+      <c r="K46" s="43"/>
+      <c r="L46" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="M46" s="76" t="s">
+      <c r="M46" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="N46" s="76"/>
-      <c r="O46" s="76" t="s">
+      <c r="N46" s="44"/>
+      <c r="O46" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="P46" s="76" t="s">
+      <c r="P46" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="Q46" s="76" t="s">
+      <c r="Q46" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="R46" s="76" t="s">
+      <c r="R46" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="S46" s="76" t="s">
+      <c r="S46" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="T46" s="76" t="s">
+      <c r="T46" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="U46" s="76" t="s">
+      <c r="U46" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="V46" s="76" t="s">
+      <c r="V46" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="W46" s="76"/>
-      <c r="X46" s="76"/>
-      <c r="Y46" s="76"/>
-      <c r="Z46" s="77"/>
-      <c r="AA46" s="74"/>
+      <c r="W46" s="44"/>
+      <c r="X46" s="44"/>
+      <c r="Y46" s="44"/>
+      <c r="Z46" s="45"/>
+      <c r="AA46" s="42"/>
     </row>
     <row r="47" spans="2:27" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B47" s="11"/>
@@ -3069,52 +3069,52 @@
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
       <c r="I47" s="11"/>
-      <c r="J47" s="70"/>
-      <c r="K47" s="78"/>
-      <c r="L47" s="66" t="s">
+      <c r="J47" s="38"/>
+      <c r="K47" s="46"/>
+      <c r="L47" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="M47" s="66" t="s">
+      <c r="M47" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="N47" s="66" t="s">
+      <c r="N47" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="O47" s="66" t="s">
+      <c r="O47" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="P47" s="66" t="s">
+      <c r="P47" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="Q47" s="66" t="s">
+      <c r="Q47" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="R47" s="66" t="s">
+      <c r="R47" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="S47" s="66" t="s">
+      <c r="S47" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="T47" s="66" t="s">
+      <c r="T47" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="U47" s="66" t="s">
+      <c r="U47" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="V47" s="66" t="s">
+      <c r="V47" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="W47" s="66" t="s">
+      <c r="W47" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="X47" s="66" t="s">
+      <c r="X47" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="Y47" s="66" t="s">
+      <c r="Y47" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="Z47" s="79"/>
-      <c r="AA47" s="74"/>
+      <c r="Z47" s="47"/>
+      <c r="AA47" s="42"/>
     </row>
     <row r="48" spans="2:27" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B48" s="11"/>
@@ -3125,46 +3125,46 @@
       <c r="G48" s="11"/>
       <c r="H48" s="11"/>
       <c r="I48" s="11"/>
-      <c r="J48" s="70"/>
-      <c r="K48" s="78"/>
-      <c r="L48" s="66" t="s">
+      <c r="J48" s="38"/>
+      <c r="K48" s="46"/>
+      <c r="L48" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="M48" s="66" t="s">
+      <c r="M48" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="N48" s="66"/>
-      <c r="O48" s="66" t="s">
+      <c r="N48" s="34"/>
+      <c r="O48" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="P48" s="66" t="s">
+      <c r="P48" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="Q48" s="66"/>
-      <c r="R48" s="66" t="s">
+      <c r="Q48" s="34"/>
+      <c r="R48" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="S48" s="66" t="s">
+      <c r="S48" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="T48" s="66" t="s">
+      <c r="T48" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="U48" s="66" t="s">
+      <c r="U48" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="V48" s="66" t="s">
+      <c r="V48" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="W48" s="66"/>
-      <c r="X48" s="66" t="s">
+      <c r="W48" s="34"/>
+      <c r="X48" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="Y48" s="66" t="s">
+      <c r="Y48" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="Z48" s="79"/>
-      <c r="AA48" s="74"/>
+      <c r="Z48" s="47"/>
+      <c r="AA48" s="42"/>
     </row>
     <row r="49" spans="1:27" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="11"/>
@@ -3175,38 +3175,38 @@
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
       <c r="I49" s="11"/>
-      <c r="J49" s="70"/>
-      <c r="K49" s="80"/>
-      <c r="L49" s="81" t="s">
+      <c r="J49" s="38"/>
+      <c r="K49" s="48"/>
+      <c r="L49" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="M49" s="81" t="s">
+      <c r="M49" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="N49" s="81" t="s">
+      <c r="N49" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="O49" s="81">
+      <c r="O49" s="49">
         <v>1</v>
       </c>
-      <c r="P49" s="81">
+      <c r="P49" s="49">
         <v>0</v>
       </c>
-      <c r="Q49" s="81">
+      <c r="Q49" s="49">
         <v>0</v>
       </c>
-      <c r="R49" s="81">
+      <c r="R49" s="49">
         <v>0</v>
       </c>
-      <c r="S49" s="81"/>
-      <c r="T49" s="81"/>
-      <c r="U49" s="81"/>
-      <c r="V49" s="81"/>
-      <c r="W49" s="81"/>
-      <c r="X49" s="81"/>
-      <c r="Y49" s="81"/>
-      <c r="Z49" s="82"/>
-      <c r="AA49" s="74"/>
+      <c r="S49" s="49"/>
+      <c r="T49" s="49"/>
+      <c r="U49" s="49"/>
+      <c r="V49" s="49"/>
+      <c r="W49" s="49"/>
+      <c r="X49" s="49"/>
+      <c r="Y49" s="49"/>
+      <c r="Z49" s="50"/>
+      <c r="AA49" s="42"/>
     </row>
     <row r="50" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="11"/>
@@ -3217,24 +3217,24 @@
       <c r="G50" s="11"/>
       <c r="H50" s="11"/>
       <c r="I50" s="11"/>
-      <c r="J50" s="70"/>
-      <c r="K50" s="83"/>
-      <c r="L50" s="83"/>
-      <c r="M50" s="83"/>
-      <c r="N50" s="83"/>
-      <c r="O50" s="83"/>
-      <c r="P50" s="83"/>
-      <c r="Q50" s="83"/>
-      <c r="R50" s="83"/>
-      <c r="S50" s="83"/>
-      <c r="T50" s="83"/>
-      <c r="U50" s="83"/>
-      <c r="V50" s="83"/>
-      <c r="W50" s="83"/>
-      <c r="X50" s="83"/>
-      <c r="Y50" s="83"/>
-      <c r="Z50" s="83"/>
-      <c r="AA50" s="74"/>
+      <c r="J50" s="38"/>
+      <c r="K50" s="51"/>
+      <c r="L50" s="51"/>
+      <c r="M50" s="51"/>
+      <c r="N50" s="51"/>
+      <c r="O50" s="51"/>
+      <c r="P50" s="51"/>
+      <c r="Q50" s="51"/>
+      <c r="R50" s="51"/>
+      <c r="S50" s="51"/>
+      <c r="T50" s="51"/>
+      <c r="U50" s="51"/>
+      <c r="V50" s="51"/>
+      <c r="W50" s="51"/>
+      <c r="X50" s="51"/>
+      <c r="Y50" s="51"/>
+      <c r="Z50" s="51"/>
+      <c r="AA50" s="42"/>
     </row>
     <row r="51" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="11"/>
@@ -3245,24 +3245,24 @@
       <c r="G51" s="11"/>
       <c r="H51" s="11"/>
       <c r="I51" s="11"/>
-      <c r="J51" s="71"/>
-      <c r="K51" s="84"/>
-      <c r="L51" s="84"/>
-      <c r="M51" s="84"/>
-      <c r="N51" s="84"/>
-      <c r="O51" s="84"/>
-      <c r="P51" s="84"/>
-      <c r="Q51" s="84"/>
-      <c r="R51" s="84"/>
-      <c r="S51" s="72"/>
-      <c r="T51" s="72"/>
-      <c r="U51" s="72"/>
-      <c r="V51" s="72"/>
-      <c r="W51" s="72"/>
-      <c r="X51" s="72"/>
-      <c r="Y51" s="72"/>
-      <c r="Z51" s="72"/>
-      <c r="AA51" s="73"/>
+      <c r="J51" s="39"/>
+      <c r="K51" s="52"/>
+      <c r="L51" s="52"/>
+      <c r="M51" s="52"/>
+      <c r="N51" s="52"/>
+      <c r="O51" s="52"/>
+      <c r="P51" s="52"/>
+      <c r="Q51" s="52"/>
+      <c r="R51" s="52"/>
+      <c r="S51" s="40"/>
+      <c r="T51" s="40"/>
+      <c r="U51" s="40"/>
+      <c r="V51" s="40"/>
+      <c r="W51" s="40"/>
+      <c r="X51" s="40"/>
+      <c r="Y51" s="40"/>
+      <c r="Z51" s="40"/>
+      <c r="AA51" s="41"/>
     </row>
     <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B52" s="11"/>
@@ -3376,58 +3376,58 @@
     </row>
     <row r="63" spans="1:27" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="28"/>
-      <c r="B63" s="85"/>
-      <c r="C63" s="85"/>
-      <c r="D63" s="85"/>
-      <c r="E63" s="85"/>
-      <c r="F63" s="85"/>
-      <c r="G63" s="85"/>
-      <c r="H63" s="85"/>
-      <c r="I63" s="85"/>
-      <c r="J63" s="91"/>
-      <c r="K63" s="91" t="s">
+      <c r="B63" s="53"/>
+      <c r="C63" s="53"/>
+      <c r="D63" s="53"/>
+      <c r="E63" s="53"/>
+      <c r="F63" s="53"/>
+      <c r="G63" s="53"/>
+      <c r="H63" s="53"/>
+      <c r="I63" s="53"/>
+      <c r="J63" s="58"/>
+      <c r="K63" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="L63" s="91"/>
-      <c r="M63" s="91"/>
-      <c r="N63" s="92"/>
+      <c r="L63" s="58"/>
+      <c r="M63" s="58"/>
+      <c r="N63" s="59"/>
     </row>
     <row r="64" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A64" s="29"/>
-      <c r="B64" s="86"/>
-      <c r="C64" s="86"/>
-      <c r="D64" s="86"/>
-      <c r="E64" s="86"/>
-      <c r="F64" s="86"/>
-      <c r="G64" s="86"/>
-      <c r="H64" s="86"/>
-      <c r="I64" s="86"/>
-      <c r="J64" s="86"/>
-      <c r="K64" s="86"/>
-      <c r="L64" s="86"/>
-      <c r="M64" s="86"/>
+      <c r="B64" s="54"/>
+      <c r="C64" s="54"/>
+      <c r="D64" s="54"/>
+      <c r="E64" s="54"/>
+      <c r="F64" s="54"/>
+      <c r="G64" s="54"/>
+      <c r="H64" s="54"/>
+      <c r="I64" s="54"/>
+      <c r="J64" s="54"/>
+      <c r="K64" s="54"/>
+      <c r="L64" s="54"/>
+      <c r="M64" s="54"/>
       <c r="N64" s="30"/>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="29"/>
-      <c r="B65" s="34" t="s">
+      <c r="B65" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="C65" s="34"/>
-      <c r="D65" s="34"/>
-      <c r="E65" s="34"/>
-      <c r="F65" s="34"/>
-      <c r="G65" s="34"/>
-      <c r="H65" s="34"/>
-      <c r="I65" s="34"/>
-      <c r="J65" s="86"/>
-      <c r="K65" s="86"/>
-      <c r="L65" s="86"/>
-      <c r="M65" s="86"/>
+      <c r="C65" s="63"/>
+      <c r="D65" s="63"/>
+      <c r="E65" s="63"/>
+      <c r="F65" s="63"/>
+      <c r="G65" s="63"/>
+      <c r="H65" s="63"/>
+      <c r="I65" s="63"/>
+      <c r="J65" s="54"/>
+      <c r="K65" s="54"/>
+      <c r="L65" s="54"/>
+      <c r="M65" s="54"/>
       <c r="N65" s="30"/>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A66" s="87" t="s">
+      <c r="A66" s="55" t="s">
         <v>19</v>
       </c>
       <c r="B66" s="6" t="s">
@@ -3454,14 +3454,14 @@
       <c r="I66" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J66" s="86"/>
-      <c r="K66" s="86"/>
-      <c r="L66" s="86"/>
-      <c r="M66" s="86"/>
+      <c r="J66" s="54"/>
+      <c r="K66" s="54"/>
+      <c r="L66" s="54"/>
+      <c r="M66" s="54"/>
       <c r="N66" s="30"/>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A67" s="88" t="s">
+      <c r="A67" s="56" t="s">
         <v>18</v>
       </c>
       <c r="B67" s="12">
@@ -3470,20 +3470,20 @@
       <c r="C67" s="12">
         <v>0</v>
       </c>
-      <c r="D67" s="35"/>
-      <c r="E67" s="36"/>
-      <c r="F67" s="36"/>
-      <c r="G67" s="36"/>
-      <c r="H67" s="36"/>
-      <c r="I67" s="37"/>
-      <c r="J67" s="86"/>
-      <c r="K67" s="86"/>
-      <c r="L67" s="86"/>
-      <c r="M67" s="86"/>
+      <c r="D67" s="64"/>
+      <c r="E67" s="65"/>
+      <c r="F67" s="65"/>
+      <c r="G67" s="65"/>
+      <c r="H67" s="65"/>
+      <c r="I67" s="66"/>
+      <c r="J67" s="54"/>
+      <c r="K67" s="54"/>
+      <c r="L67" s="54"/>
+      <c r="M67" s="54"/>
       <c r="N67" s="30"/>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A68" s="88" t="s">
+      <c r="A68" s="56" t="s">
         <v>16</v>
       </c>
       <c r="B68" s="12">
@@ -3492,20 +3492,20 @@
       <c r="C68" s="12">
         <v>1</v>
       </c>
-      <c r="D68" s="38"/>
-      <c r="E68" s="39"/>
-      <c r="F68" s="39"/>
-      <c r="G68" s="39"/>
-      <c r="H68" s="39"/>
-      <c r="I68" s="40"/>
-      <c r="J68" s="86"/>
-      <c r="K68" s="86"/>
-      <c r="L68" s="86"/>
-      <c r="M68" s="86"/>
+      <c r="D68" s="67"/>
+      <c r="E68" s="68"/>
+      <c r="F68" s="68"/>
+      <c r="G68" s="68"/>
+      <c r="H68" s="68"/>
+      <c r="I68" s="69"/>
+      <c r="J68" s="54"/>
+      <c r="K68" s="54"/>
+      <c r="L68" s="54"/>
+      <c r="M68" s="54"/>
       <c r="N68" s="30"/>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A69" s="88" t="s">
+      <c r="A69" s="56" t="s">
         <v>17</v>
       </c>
       <c r="B69" s="12">
@@ -3514,124 +3514,124 @@
       <c r="C69" s="12">
         <v>0</v>
       </c>
-      <c r="D69" s="41"/>
-      <c r="E69" s="42"/>
-      <c r="F69" s="42"/>
-      <c r="G69" s="42"/>
-      <c r="H69" s="42"/>
-      <c r="I69" s="43"/>
-      <c r="J69" s="86"/>
-      <c r="K69" s="86"/>
-      <c r="L69" s="86"/>
-      <c r="M69" s="86"/>
+      <c r="D69" s="70"/>
+      <c r="E69" s="71"/>
+      <c r="F69" s="71"/>
+      <c r="G69" s="71"/>
+      <c r="H69" s="71"/>
+      <c r="I69" s="72"/>
+      <c r="J69" s="54"/>
+      <c r="K69" s="54"/>
+      <c r="L69" s="54"/>
+      <c r="M69" s="54"/>
       <c r="N69" s="30"/>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="29"/>
-      <c r="B70" s="89" t="s">
+      <c r="B70" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="C70" s="89"/>
-      <c r="D70" s="89"/>
-      <c r="E70" s="89"/>
-      <c r="F70" s="89"/>
-      <c r="G70" s="89"/>
-      <c r="H70" s="89"/>
-      <c r="I70" s="89"/>
-      <c r="J70" s="86"/>
-      <c r="K70" s="86"/>
-      <c r="L70" s="86"/>
-      <c r="M70" s="86"/>
+      <c r="C70" s="60"/>
+      <c r="D70" s="60"/>
+      <c r="E70" s="60"/>
+      <c r="F70" s="60"/>
+      <c r="G70" s="60"/>
+      <c r="H70" s="60"/>
+      <c r="I70" s="60"/>
+      <c r="J70" s="54"/>
+      <c r="K70" s="54"/>
+      <c r="L70" s="54"/>
+      <c r="M70" s="54"/>
       <c r="N70" s="30"/>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="29"/>
-      <c r="B71" s="90" t="s">
+      <c r="B71" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="C71" s="86"/>
-      <c r="D71" s="86"/>
-      <c r="E71" s="86"/>
-      <c r="F71" s="86"/>
-      <c r="G71" s="86"/>
-      <c r="H71" s="86"/>
-      <c r="I71" s="86"/>
-      <c r="J71" s="86"/>
-      <c r="K71" s="86"/>
-      <c r="L71" s="86"/>
-      <c r="M71" s="86"/>
+      <c r="C71" s="54"/>
+      <c r="D71" s="54"/>
+      <c r="E71" s="54"/>
+      <c r="F71" s="54"/>
+      <c r="G71" s="54"/>
+      <c r="H71" s="54"/>
+      <c r="I71" s="54"/>
+      <c r="J71" s="54"/>
+      <c r="K71" s="54"/>
+      <c r="L71" s="54"/>
+      <c r="M71" s="54"/>
       <c r="N71" s="30"/>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="29"/>
-      <c r="B72" s="86" t="s">
+      <c r="B72" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="C72" s="86"/>
-      <c r="D72" s="86"/>
-      <c r="E72" s="86"/>
-      <c r="F72" s="86"/>
-      <c r="G72" s="86"/>
-      <c r="H72" s="86"/>
-      <c r="I72" s="86"/>
-      <c r="J72" s="86"/>
-      <c r="K72" s="86"/>
-      <c r="L72" s="86"/>
-      <c r="M72" s="86"/>
+      <c r="C72" s="54"/>
+      <c r="D72" s="54"/>
+      <c r="E72" s="54"/>
+      <c r="F72" s="54"/>
+      <c r="G72" s="54"/>
+      <c r="H72" s="54"/>
+      <c r="I72" s="54"/>
+      <c r="J72" s="54"/>
+      <c r="K72" s="54"/>
+      <c r="L72" s="54"/>
+      <c r="M72" s="54"/>
       <c r="N72" s="30"/>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="29"/>
-      <c r="B73" s="86" t="s">
+      <c r="B73" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="C73" s="86"/>
-      <c r="D73" s="86"/>
-      <c r="E73" s="86"/>
-      <c r="F73" s="86"/>
-      <c r="G73" s="86"/>
-      <c r="H73" s="86"/>
-      <c r="I73" s="86"/>
-      <c r="J73" s="86"/>
-      <c r="K73" s="86"/>
-      <c r="L73" s="86"/>
-      <c r="M73" s="86"/>
+      <c r="C73" s="54"/>
+      <c r="D73" s="54"/>
+      <c r="E73" s="54"/>
+      <c r="F73" s="54"/>
+      <c r="G73" s="54"/>
+      <c r="H73" s="54"/>
+      <c r="I73" s="54"/>
+      <c r="J73" s="54"/>
+      <c r="K73" s="54"/>
+      <c r="L73" s="54"/>
+      <c r="M73" s="54"/>
       <c r="N73" s="30"/>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="29"/>
-      <c r="B74" s="86" t="s">
+      <c r="B74" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="C74" s="86"/>
-      <c r="D74" s="86"/>
-      <c r="E74" s="86"/>
-      <c r="F74" s="86"/>
-      <c r="G74" s="86"/>
-      <c r="H74" s="86"/>
-      <c r="I74" s="86"/>
-      <c r="J74" s="86"/>
-      <c r="K74" s="86"/>
-      <c r="L74" s="86"/>
-      <c r="M74" s="86"/>
+      <c r="C74" s="54"/>
+      <c r="D74" s="54"/>
+      <c r="E74" s="54"/>
+      <c r="F74" s="54"/>
+      <c r="G74" s="54"/>
+      <c r="H74" s="54"/>
+      <c r="I74" s="54"/>
+      <c r="J74" s="54"/>
+      <c r="K74" s="54"/>
+      <c r="L74" s="54"/>
+      <c r="M74" s="54"/>
       <c r="N74" s="30"/>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="29"/>
-      <c r="B75" s="86" t="s">
+      <c r="B75" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="C75" s="86"/>
-      <c r="D75" s="86"/>
-      <c r="E75" s="86"/>
-      <c r="F75" s="86"/>
-      <c r="G75" s="86"/>
-      <c r="H75" s="86"/>
-      <c r="I75" s="86"/>
-      <c r="J75" s="86"/>
-      <c r="K75" s="86"/>
-      <c r="L75" s="86"/>
-      <c r="M75" s="86"/>
+      <c r="C75" s="54"/>
+      <c r="D75" s="54"/>
+      <c r="E75" s="54"/>
+      <c r="F75" s="54"/>
+      <c r="G75" s="54"/>
+      <c r="H75" s="54"/>
+      <c r="I75" s="54"/>
+      <c r="J75" s="54"/>
+      <c r="K75" s="54"/>
+      <c r="L75" s="54"/>
+      <c r="M75" s="54"/>
       <c r="N75" s="30"/>
     </row>
     <row r="76" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>